<commit_message>
Adiciona revisao do leiaute da tabela no excel
</commit_message>
<xml_diff>
--- a/static/leiaute-tabelas-covid19.xlsx
+++ b/static/leiaute-tabelas-covid19.xlsx
@@ -1,30 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10308"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Silviana\Documents\tele-trabalho\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fjunior/Local/github/transparencia-mg/especificacoes-portal-transparencia/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5467296D-39E8-3F4B-B11E-D6D77D463844}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9600"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabela" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
   <si>
     <t>TOTAL GERAL:</t>
   </si>
@@ -32,9 +41,6 @@
     <t>Número do Processo de Compra</t>
   </si>
   <si>
-    <t>Objeto/Justificativa</t>
-  </si>
-  <si>
     <t>Órgão Demandante</t>
   </si>
   <si>
@@ -68,9 +74,6 @@
     <t>0250073 000003/2020</t>
   </si>
   <si>
-    <t>Data da Publicação do Contrato</t>
-  </si>
-  <si>
     <t>Edital</t>
   </si>
   <si>
@@ -92,20 +95,44 @@
     <t>Em Andamento</t>
   </si>
   <si>
-    <t>Fim da Vigência  do Contrato</t>
-  </si>
-  <si>
     <t>CINCO - CONFIANCA INDUSTRIA E COMERCIO LTDA</t>
+  </si>
+  <si>
+    <t>Início da Vigência</t>
+  </si>
+  <si>
+    <t>Data de Publicação</t>
+  </si>
+  <si>
+    <t>Fim da Vigência Atualizado</t>
+  </si>
+  <si>
+    <t>Fim da Vigência</t>
+  </si>
+  <si>
+    <t>Objeto</t>
+  </si>
+  <si>
+    <t>Data de Cadastramento do Processo</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>Código Órgão</t>
+  </si>
+  <si>
+    <t>Código Órgão Demandante</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -151,6 +178,12 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
@@ -269,7 +302,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -295,43 +328,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Vírgula" xfId="1" builtinId="3"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -357,13 +393,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>691243</xdr:colOff>
+      <xdr:colOff>860577</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>68036</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Imagem 2"/>
+        <xdr:cNvPr id="3" name="Imagem 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -387,20 +429,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>930730</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>443592</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1269397</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>627037</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>1179500</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>672192</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1518167</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>855637</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="10" name="Imagem 9"/>
+        <xdr:cNvPr id="10" name="Imagem 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -413,7 +461,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7380516" y="2348592"/>
+          <a:off x="11697508" y="2602593"/>
           <a:ext cx="248770" cy="228600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -432,13 +480,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>404132</xdr:colOff>
+      <xdr:colOff>573466</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>178023</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Imagem 3"/>
+        <xdr:cNvPr id="4" name="Imagem 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -462,15 +516,21 @@
   </xdr:twoCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>1035050</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>574675</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>1303161</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>645231</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="248770" cy="228600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="15" name="Imagem 14"/>
+        <xdr:cNvPr id="15" name="Imagem 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -483,7 +543,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17594943" y="2479675"/>
+          <a:off x="27168828" y="2620787"/>
           <a:ext cx="248770" cy="228600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -495,20 +555,26 @@
   </xdr:oneCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>190501</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>1325103</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>3153</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Imagem 4"/>
+        <xdr:cNvPr id="5" name="Imagem 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -533,20 +599,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>870857</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>136072</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>1160513</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>65627</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Imagem 7"/>
+        <xdr:cNvPr id="8" name="Imagem 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -571,7 +643,7 @@
   </xdr:twoCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>1352551</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -579,7 +651,13 @@
     <xdr:ext cx="248770" cy="228600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="16" name="Imagem 15"/>
+        <xdr:cNvPr id="16" name="Imagem 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000010000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -604,7 +682,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>1476375</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -612,7 +690,13 @@
     <xdr:ext cx="248770" cy="228600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="17" name="Imagem 16"/>
+        <xdr:cNvPr id="17" name="Imagem 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000011000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -645,7 +729,13 @@
     <xdr:ext cx="248770" cy="228600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="18" name="Imagem 17"/>
+        <xdr:cNvPr id="18" name="Imagem 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000012000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -670,7 +760,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>828675</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -678,7 +768,13 @@
     <xdr:ext cx="248770" cy="228600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="19" name="Imagem 18"/>
+        <xdr:cNvPr id="19" name="Imagem 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000013000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -703,15 +799,21 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>1382033</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>423182</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>1720699</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>592515</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="248770" cy="228600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="20" name="Imagem 19"/>
+        <xdr:cNvPr id="20" name="Imagem 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000014000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -724,7 +826,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="16213819" y="2328182"/>
+          <a:off x="25610810" y="2568071"/>
           <a:ext cx="248770" cy="228600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -736,20 +838,26 @@
   </xdr:oneCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>810988</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>364670</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>1107321</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>604559</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>1059758</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>593270</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>15536</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>833159</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="27" name="Imagem 26"/>
+        <xdr:cNvPr id="27" name="Imagem 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -762,7 +870,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14921595" y="2269670"/>
+          <a:off x="23656877" y="2580115"/>
           <a:ext cx="248770" cy="228600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -774,20 +882,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>800101</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>489856</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>1166990</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>616856</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>1048871</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>718456</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>4648</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>845456</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="28" name="Imagem 27"/>
+        <xdr:cNvPr id="28" name="Imagem 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -800,7 +914,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13862958" y="2394856"/>
+          <a:off x="22305434" y="2592412"/>
           <a:ext cx="248770" cy="228600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -812,20 +926,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>911681</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>478971</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>1081014</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>605971</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>1160451</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>707571</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>1329784</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>834571</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="29" name="Imagem 28"/>
+        <xdr:cNvPr id="29" name="Imagem 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -838,7 +958,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12396110" y="2383971"/>
+          <a:off x="20850681" y="2581527"/>
           <a:ext cx="248770" cy="228600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -850,20 +970,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>710295</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>563335</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>1034851</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>633891</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>959065</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>791935</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>1283621</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>862491</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="30" name="Imagem 29"/>
+        <xdr:cNvPr id="30" name="Imagem 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -876,7 +1002,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10779581" y="2468335"/>
+          <a:off x="16782851" y="2609447"/>
           <a:ext cx="248770" cy="228600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -888,20 +1014,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>685802</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>484413</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1052691</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>639636</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>934572</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>713013</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1301461</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>868236</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="31" name="Imagem 30"/>
+        <xdr:cNvPr id="31" name="Imagem 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -914,7 +1046,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9965873" y="2389413"/>
+          <a:off x="15460135" y="2615192"/>
           <a:ext cx="248770" cy="228600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -926,20 +1058,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>715736</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>459920</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>927403</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>601031</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>964506</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>688520</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1176173</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>829631</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="32" name="Imagem 31"/>
+        <xdr:cNvPr id="32" name="Imagem 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000020000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -952,7 +1090,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8580665" y="2364920"/>
+          <a:off x="12964181" y="2576587"/>
           <a:ext cx="248770" cy="228600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -964,20 +1102,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1153887</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1351442</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>639535</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1402657</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1600212</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>868135</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="33" name="Imagem 32"/>
+        <xdr:cNvPr id="33" name="Imagem 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000021000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -990,7 +1134,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6188530" y="2544535"/>
+          <a:off x="10156775" y="2615091"/>
           <a:ext cx="248770" cy="228600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1002,20 +1146,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>898073</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>451756</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1180295</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>635200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1146843</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>680356</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1429065</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>863800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="34" name="Imagem 33"/>
+        <xdr:cNvPr id="34" name="Imagem 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000022000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1028,7 +1178,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3823609" y="2356756"/>
+          <a:off x="7572628" y="2610756"/>
           <a:ext cx="248770" cy="228600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1040,20 +1190,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>1023259</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>522513</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>1272029</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>751113</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="35" name="Imagem 34"/>
+        <xdr:cNvPr id="35" name="Imagem 34">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1341,33 +1497,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B6:O15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B6:T15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.5703125" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" customWidth="1"/>
-    <col min="4" max="4" width="19" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" customWidth="1"/>
-    <col min="6" max="6" width="21.28515625" customWidth="1"/>
-    <col min="7" max="7" width="21.140625" customWidth="1"/>
-    <col min="8" max="8" width="15.42578125" customWidth="1"/>
-    <col min="9" max="9" width="17.5703125" customWidth="1"/>
-    <col min="10" max="10" width="17.42578125" customWidth="1"/>
-    <col min="11" max="11" width="18" customWidth="1"/>
-    <col min="12" max="12" width="18.5703125" customWidth="1"/>
-    <col min="13" max="13" width="17.5703125" customWidth="1"/>
-    <col min="14" max="14" width="26" customWidth="1"/>
-    <col min="15" max="15" width="20.42578125" customWidth="1"/>
+    <col min="1" max="1" width="3.5" customWidth="1"/>
+    <col min="2" max="3" width="20.5" customWidth="1"/>
+    <col min="4" max="5" width="19.6640625" customWidth="1"/>
+    <col min="6" max="6" width="19" customWidth="1"/>
+    <col min="7" max="7" width="12.5" customWidth="1"/>
+    <col min="8" max="8" width="21.33203125" customWidth="1"/>
+    <col min="9" max="9" width="21.1640625" customWidth="1"/>
+    <col min="10" max="11" width="15.5" customWidth="1"/>
+    <col min="12" max="15" width="17.5" customWidth="1"/>
+    <col min="16" max="16" width="18" customWidth="1"/>
+    <col min="17" max="17" width="18.5" customWidth="1"/>
+    <col min="18" max="18" width="17.5" customWidth="1"/>
+    <col min="19" max="19" width="26" customWidth="1"/>
+    <col min="20" max="20" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:20">
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -1381,8 +1536,13 @@
       <c r="L6" s="5"/>
       <c r="M6" s="5"/>
       <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="5"/>
+      <c r="S6" s="5"/>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:20">
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -1396,8 +1556,13 @@
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>
       <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="5"/>
+      <c r="R7" s="5"/>
+      <c r="S7" s="5"/>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:20">
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -1411,8 +1576,13 @@
       <c r="L8" s="5"/>
       <c r="M8" s="5"/>
       <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="5"/>
+      <c r="S8" s="5"/>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:20">
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -1426,8 +1596,13 @@
       <c r="L9" s="5"/>
       <c r="M9" s="5"/>
       <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="5"/>
+      <c r="S9" s="5"/>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:20">
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -1441,167 +1616,206 @@
       <c r="L10" s="5"/>
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="5"/>
+      <c r="R10" s="5"/>
+      <c r="S10" s="5"/>
     </row>
-    <row r="11" spans="2:15" s="8" customFormat="1" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:20" s="8" customFormat="1" ht="72" customHeight="1" thickBot="1">
       <c r="B11" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C11" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="G11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="K11" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="L11" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="M11" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N11" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="O11" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P11" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q11" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="R11" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="S11" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="T11" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="2:20" ht="72" customHeight="1" thickTop="1">
+      <c r="B12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="11"/>
+      <c r="F12" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="H12" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="I12" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="J12" s="20">
+        <v>995060</v>
+      </c>
+      <c r="K12" s="20"/>
+      <c r="L12" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="M12" s="16">
+        <v>43939</v>
+      </c>
+      <c r="N12" s="16"/>
+      <c r="O12" s="16"/>
+      <c r="P12" s="16">
+        <v>44196</v>
+      </c>
+      <c r="Q12" s="17">
+        <v>5075964000112</v>
+      </c>
+      <c r="R12" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="S12" s="10">
+        <v>2000000</v>
+      </c>
+      <c r="T12" s="10">
+        <v>2000000</v>
+      </c>
+    </row>
+    <row r="13" spans="2:20" ht="76.5" customHeight="1" thickBot="1">
+      <c r="B13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="11"/>
+      <c r="F13" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="H13" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="I13" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="I11" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="J11" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="K11" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="L11" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="M11" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="N11" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="O11" s="7" t="s">
-        <v>5</v>
+      <c r="J13" s="20">
+        <v>905095</v>
+      </c>
+      <c r="K13" s="20"/>
+      <c r="L13" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="M13" s="16">
+        <v>43941</v>
+      </c>
+      <c r="N13" s="16"/>
+      <c r="O13" s="16"/>
+      <c r="P13" s="16">
+        <v>80782</v>
+      </c>
+      <c r="Q13" s="17">
+        <v>5075964000112</v>
+      </c>
+      <c r="R13" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="S13" s="10">
+        <v>158600000</v>
+      </c>
+      <c r="T13" s="10">
+        <v>158600000</v>
       </c>
     </row>
-    <row r="12" spans="2:15" ht="72" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="E12" s="14"/>
-      <c r="F12" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="G12" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="H12" s="17">
-        <v>995060</v>
-      </c>
-      <c r="I12" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="J12" s="18">
-        <v>43939</v>
-      </c>
-      <c r="K12" s="18">
-        <v>44196</v>
-      </c>
-      <c r="L12" s="19">
-        <v>5075964000112</v>
-      </c>
-      <c r="M12" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="N12" s="11">
-        <v>2000000</v>
-      </c>
-      <c r="O12" s="11">
-        <v>2000000</v>
-      </c>
-    </row>
-    <row r="13" spans="2:15" ht="76.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13" s="14"/>
-      <c r="F13" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="G13" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="H13" s="17">
-        <v>905095</v>
-      </c>
-      <c r="I13" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="J13" s="18">
-        <v>43941</v>
-      </c>
-      <c r="K13" s="18">
-        <v>80782</v>
-      </c>
-      <c r="L13" s="19">
-        <v>5075964000112</v>
-      </c>
-      <c r="M13" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="N13" s="11">
-        <v>158600000</v>
-      </c>
-      <c r="O13" s="11">
-        <v>158600000</v>
-      </c>
-    </row>
-    <row r="14" spans="2:15" ht="30.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="9" t="s">
+    <row r="14" spans="2:20" ht="30.75" customHeight="1" thickTop="1">
+      <c r="B14" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="3">
-        <f>SUM(G12:G13)</f>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="3">
+        <f>SUM(I12:I13)</f>
         <v>0</v>
       </c>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
       <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
+      <c r="K14" s="9"/>
       <c r="L14" s="6"/>
       <c r="M14" s="6"/>
-      <c r="N14" s="3">
-        <f>SUM(N12:N13)</f>
+      <c r="N14" s="9"/>
+      <c r="O14" s="9"/>
+      <c r="P14" s="6"/>
+      <c r="Q14" s="6"/>
+      <c r="R14" s="6"/>
+      <c r="S14" s="3">
+        <f>SUM(S12:S13)</f>
         <v>160600000</v>
       </c>
-      <c r="O14" s="3">
-        <f>SUM(O12:O13)</f>
+      <c r="T14" s="3">
+        <f>SUM(T12:T13)</f>
         <v>160600000</v>
       </c>
     </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:20">
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
@@ -1611,10 +1825,15 @@
       <c r="L15" s="5"/>
       <c r="M15" s="5"/>
       <c r="N15" s="5"/>
+      <c r="O15" s="5"/>
+      <c r="P15" s="5"/>
+      <c r="Q15" s="5"/>
+      <c r="R15" s="5"/>
+      <c r="S15" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B14:F14"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
corrigi imagem layout do painel
</commit_message>
<xml_diff>
--- a/static/leiaute-tabelas-covid19.xlsx
+++ b/static/leiaute-tabelas-covid19.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Silviana\Documents\tele-trabalho\GIT\especificacoes-portal-transparencia\static\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Silviana\Documents\1.CGE\tele-trabalho\GIT\especificacoes-portal-transparencia\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
   <si>
     <t>TOTAL GERAL:</t>
   </si>
@@ -120,6 +120,10 @@
   <si>
     <t>Código 
 Órgão Demandante</t>
+  </si>
+  <si>
+    <t>Código 
+Órgão Contrato</t>
   </si>
 </sst>
 </file>
@@ -129,7 +133,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -146,42 +150,38 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Verdana"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFC00000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
-      <name val="Verdana"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFC00000"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Segoe UI"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -299,66 +299,55 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -392,7 +381,7 @@
       <xdr:col>7</xdr:col>
       <xdr:colOff>987577</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>68036</xdr:rowOff>
+      <xdr:rowOff>122011</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -434,8 +423,8 @@
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>700466</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>178023</xdr:rowOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>238348</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -509,15 +498,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>190501</xdr:colOff>
+      <xdr:colOff>761999</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>1308170</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>6419</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>3153</xdr:rowOff>
+      <xdr:rowOff>2085</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -540,8 +529,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14260287" y="0"/>
-          <a:ext cx="2869512" cy="1908153"/>
+          <a:off x="19732624" y="1"/>
+          <a:ext cx="2498795" cy="1589584"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -561,7 +550,7 @@
       <xdr:col>19</xdr:col>
       <xdr:colOff>1143580</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>65627</xdr:rowOff>
+      <xdr:rowOff>132302</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1350,8 +1339,8 @@
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>108822</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>152369</xdr:rowOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>15844</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1646,340 +1635,341 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B6:T15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="X12" sqref="W12:X12"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="W8" sqref="W8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.42578125" customWidth="1"/>
-    <col min="2" max="3" width="20.42578125" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" customWidth="1"/>
-    <col min="5" max="6" width="15.140625" customWidth="1"/>
-    <col min="7" max="7" width="19" customWidth="1"/>
-    <col min="8" max="8" width="15.140625" customWidth="1"/>
-    <col min="9" max="9" width="16" customWidth="1"/>
-    <col min="10" max="11" width="15.42578125" customWidth="1"/>
-    <col min="12" max="12" width="17.42578125" customWidth="1"/>
-    <col min="13" max="13" width="13.7109375" customWidth="1"/>
-    <col min="14" max="14" width="14.5703125" customWidth="1"/>
-    <col min="15" max="15" width="11.42578125" customWidth="1"/>
-    <col min="16" max="16" width="12.42578125" customWidth="1"/>
-    <col min="17" max="17" width="18.42578125" customWidth="1"/>
-    <col min="18" max="18" width="17.42578125" customWidth="1"/>
-    <col min="19" max="19" width="26.42578125" customWidth="1"/>
-    <col min="20" max="20" width="22.42578125" customWidth="1"/>
-    <col min="21" max="21" width="2" customWidth="1"/>
+    <col min="1" max="1" width="3.42578125" style="2" customWidth="1"/>
+    <col min="2" max="3" width="20.42578125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" style="2" customWidth="1"/>
+    <col min="5" max="6" width="15.140625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="19" style="2" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="16" style="2" customWidth="1"/>
+    <col min="10" max="11" width="15.42578125" style="2" customWidth="1"/>
+    <col min="12" max="12" width="17.42578125" style="2" customWidth="1"/>
+    <col min="13" max="13" width="13.7109375" style="2" customWidth="1"/>
+    <col min="14" max="14" width="14.5703125" style="2" customWidth="1"/>
+    <col min="15" max="15" width="11.42578125" style="2" customWidth="1"/>
+    <col min="16" max="16" width="16" style="2" customWidth="1"/>
+    <col min="17" max="17" width="18.42578125" style="2" customWidth="1"/>
+    <col min="18" max="18" width="17.42578125" style="2" customWidth="1"/>
+    <col min="19" max="19" width="26.42578125" style="2" customWidth="1"/>
+    <col min="20" max="20" width="22.42578125" style="2" customWidth="1"/>
+    <col min="21" max="21" width="2" style="2" customWidth="1"/>
+    <col min="22" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="6" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
-      <c r="P6" s="5"/>
-      <c r="Q6" s="5"/>
-      <c r="R6" s="5"/>
-      <c r="S6" s="5"/>
+    <row r="6" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
     </row>
-    <row r="7" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="5"/>
-      <c r="P7" s="5"/>
-      <c r="Q7" s="5"/>
-      <c r="R7" s="5"/>
-      <c r="S7" s="5"/>
+    <row r="7" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
     </row>
-    <row r="8" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="5"/>
-      <c r="P8" s="5"/>
-      <c r="Q8" s="5"/>
-      <c r="R8" s="5"/>
-      <c r="S8" s="5"/>
+    <row r="8" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
     </row>
-    <row r="9" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
-      <c r="O9" s="5"/>
-      <c r="P9" s="5"/>
-      <c r="Q9" s="5"/>
-      <c r="R9" s="5"/>
-      <c r="S9" s="5"/>
+    <row r="9" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
     </row>
-    <row r="10" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="5"/>
-      <c r="P10" s="5"/>
-      <c r="Q10" s="5"/>
-      <c r="R10" s="5"/>
-      <c r="S10" s="5"/>
+    <row r="10" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
     </row>
-    <row r="11" spans="2:20" s="8" customFormat="1" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="7" t="s">
+    <row r="11" spans="2:20" s="4" customFormat="1" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="F11" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="G11" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="H11" s="7" t="s">
+      <c r="H11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I11" s="7" t="s">
+      <c r="I11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="J11" s="7" t="s">
+      <c r="J11" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="K11" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="L11" s="7" t="s">
+      <c r="K11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="L11" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="M11" s="7" t="s">
+      <c r="M11" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="N11" s="7" t="s">
+      <c r="N11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="O11" s="7" t="s">
+      <c r="O11" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="P11" s="7" t="s">
+      <c r="P11" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="Q11" s="7" t="s">
+      <c r="Q11" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="R11" s="7" t="s">
+      <c r="R11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="S11" s="7" t="s">
+      <c r="S11" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="T11" s="7" t="s">
+      <c r="T11" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="2:20" ht="72" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
+    <row r="12" spans="2:20" ht="72" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="11" t="s">
+      <c r="C12" s="5"/>
+      <c r="D12" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="13" t="s">
+      <c r="E12" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13" t="s">
+      <c r="F12" s="7"/>
+      <c r="G12" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="H12" s="14" t="s">
+      <c r="H12" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="I12" s="15" t="s">
+      <c r="I12" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="J12" s="18">
+      <c r="J12" s="10">
         <v>995060</v>
       </c>
-      <c r="K12" s="18"/>
-      <c r="L12" s="13" t="s">
+      <c r="K12" s="10"/>
+      <c r="L12" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="M12" s="16">
+      <c r="M12" s="11">
         <v>43939</v>
       </c>
-      <c r="N12" s="16"/>
-      <c r="O12" s="16"/>
-      <c r="P12" s="16">
+      <c r="N12" s="11"/>
+      <c r="O12" s="11"/>
+      <c r="P12" s="11">
         <v>44196</v>
       </c>
-      <c r="Q12" s="17">
+      <c r="Q12" s="12">
         <v>5075964000112</v>
       </c>
-      <c r="R12" s="12" t="s">
+      <c r="R12" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="S12" s="10">
+      <c r="S12" s="9">
         <v>2000000</v>
       </c>
-      <c r="T12" s="10">
+      <c r="T12" s="9">
         <v>2000000</v>
       </c>
     </row>
-    <row r="13" spans="2:20" ht="76.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="2" t="s">
+    <row r="13" spans="2:20" ht="76.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="11" t="s">
+      <c r="C13" s="13"/>
+      <c r="D13" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="13" t="s">
+      <c r="E13" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13" t="s">
+      <c r="F13" s="7"/>
+      <c r="G13" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="H13" s="14" t="s">
+      <c r="H13" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="I13" s="15" t="s">
+      <c r="I13" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="J13" s="18">
+      <c r="J13" s="10">
         <v>905095</v>
       </c>
-      <c r="K13" s="18"/>
-      <c r="L13" s="13" t="s">
+      <c r="K13" s="10"/>
+      <c r="L13" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="M13" s="16">
+      <c r="M13" s="11">
         <v>43941</v>
       </c>
-      <c r="N13" s="16"/>
-      <c r="O13" s="16"/>
-      <c r="P13" s="16">
+      <c r="N13" s="11"/>
+      <c r="O13" s="11"/>
+      <c r="P13" s="11">
         <v>80782</v>
       </c>
-      <c r="Q13" s="17">
+      <c r="Q13" s="12">
         <v>5075964000112</v>
       </c>
-      <c r="R13" s="12" t="s">
+      <c r="R13" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="S13" s="10">
+      <c r="S13" s="9">
         <v>158600000</v>
       </c>
-      <c r="T13" s="10">
+      <c r="T13" s="9">
         <v>158600000</v>
       </c>
     </row>
-    <row r="14" spans="2:20" ht="30.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="19" t="s">
+    <row r="14" spans="2:20" ht="30.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="3">
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="16">
         <f>SUM(I12:I13)</f>
         <v>0</v>
       </c>
-      <c r="J14" s="6"/>
-      <c r="K14" s="20"/>
-      <c r="L14" s="6"/>
-      <c r="M14" s="6"/>
-      <c r="N14" s="9"/>
-      <c r="O14" s="9"/>
-      <c r="P14" s="6"/>
-      <c r="Q14" s="6"/>
-      <c r="R14" s="6"/>
-      <c r="S14" s="3">
+      <c r="J14" s="15"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="15"/>
+      <c r="M14" s="15"/>
+      <c r="N14" s="15"/>
+      <c r="O14" s="15"/>
+      <c r="P14" s="15"/>
+      <c r="Q14" s="15"/>
+      <c r="R14" s="15"/>
+      <c r="S14" s="16">
         <f>SUM(S12:S13)</f>
         <v>160600000</v>
       </c>
-      <c r="T14" s="3">
+      <c r="T14" s="16">
         <f>SUM(T12:T13)</f>
         <v>160600000</v>
       </c>
     </row>
-    <row r="15" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="5"/>
-      <c r="N15" s="5"/>
-      <c r="O15" s="5"/>
-      <c r="P15" s="5"/>
-      <c r="Q15" s="5"/>
-      <c r="R15" s="5"/>
-      <c r="S15" s="5"/>
+    <row r="15" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>